<commit_message>
x1246 Bio risk number in section registration
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/reg_empty.xlsx
+++ b/src/test/resources/testdata/reg_empty.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dr6/Code/stan/core/src/test/resources/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86BDF6D7-4C66-F841-A6A4-34E1F2A76081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30331725-DA1F-4449-91D2-882862F2EFDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="500" windowWidth="27640" windowHeight="15900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1160" yWindow="500" windowWidth="27640" windowHeight="15900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
   <si>
     <r>
       <t xml:space="preserve">SGP number
@@ -414,6 +414,12 @@
   </si>
   <si>
     <t>risk1</t>
+  </si>
+  <si>
+    <t>Biological risk assessment number</t>
+  </si>
+  <si>
+    <t>RISKX</t>
   </si>
 </sst>
 </file>
@@ -967,7 +973,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -1083,16 +1089,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B1:R3"/>
+  <dimension ref="B1:S3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="2:18" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:18" ht="115" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:19" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:19" ht="115" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1121,31 +1127,34 @@
         <v>8</v>
       </c>
       <c r="K2" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="L2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="M2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="N2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="O2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="Q2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="R2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="S2" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:18" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:19" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
         <v>17</v>
       </c>
@@ -1174,23 +1183,26 @@
         <v>25</v>
       </c>
       <c r="K3" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="L3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="M3" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="M3" s="12">
+      <c r="N3" s="12">
         <v>23</v>
       </c>
-      <c r="N3" s="12">
+      <c r="O3" s="12">
         <v>1</v>
       </c>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12">
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12">
         <v>4</v>
       </c>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="10">
+      <c r="R3" s="12"/>
+      <c r="S3" s="10">
         <v>10</v>
       </c>
     </row>

</xml_diff>